<commit_message>
add more details kv, breaker_id.
</commit_message>
<xml_diff>
--- a/powerapp/data/ufls_assignment.xlsx
+++ b/powerapp/data/ufls_assignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myIjat\Job\1_Operation\Network\System_Defences\UFLS_UVLS\2025_Review\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myIjat\Dojo\work\power_app\powerapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4DDD73-2B3B-4AEA-9F22-6739C94A82BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D248731-776A-4223-B4AC-D539889FE56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{EAAC684E-7C1B-4F2F-BC7C-B97D8EF3A83B}"/>
+    <workbookView xWindow="-11050" yWindow="-20840" windowWidth="17810" windowHeight="15370" xr2:uid="{EAAC684E-7C1B-4F2F-BC7C-B97D8EF3A83B}"/>
   </bookViews>
   <sheets>
     <sheet name="ufls_assignment" sheetId="1" r:id="rId1"/>
@@ -1025,10 +1025,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F1E9AA-42FA-48CE-9C0D-6753CE8DE448}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C607"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F184" sqref="F184"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1049,7 +1050,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" hidden="1">
       <c r="A2" s="4" t="s">
         <v>172</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" hidden="1">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -1223,7 +1224,7 @@
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" hidden="1">
       <c r="A18" s="4" t="s">
         <v>1</v>
       </c>
@@ -1232,7 +1233,7 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" hidden="1">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
@@ -1241,7 +1242,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" hidden="1">
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
@@ -1250,7 +1251,7 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" hidden="1">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1259,7 +1260,7 @@
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" hidden="1">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="6" customFormat="1">
+    <row r="24" spans="1:3" s="6" customFormat="1" hidden="1">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -1288,7 +1289,7 @@
       </c>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" s="6" customFormat="1">
+    <row r="25" spans="1:3" s="6" customFormat="1" hidden="1">
       <c r="A25" s="4" t="s">
         <v>8</v>
       </c>
@@ -1297,7 +1298,7 @@
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" s="7" customFormat="1">
+    <row r="26" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -1306,7 +1307,7 @@
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" s="7" customFormat="1">
+    <row r="27" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A27" s="4" t="s">
         <v>10</v>
       </c>
@@ -1315,7 +1316,7 @@
       </c>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" s="7" customFormat="1">
+    <row r="28" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
@@ -1324,7 +1325,7 @@
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" s="7" customFormat="1">
+    <row r="29" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A29" s="4" t="s">
         <v>12</v>
       </c>
@@ -1333,7 +1334,7 @@
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" hidden="1">
       <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
@@ -1342,7 +1343,7 @@
       </c>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" hidden="1">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
@@ -1351,7 +1352,7 @@
       </c>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" hidden="1">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
@@ -1360,7 +1361,7 @@
       </c>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" hidden="1">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -1369,7 +1370,7 @@
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" hidden="1">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
@@ -1378,7 +1379,7 @@
       </c>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" hidden="1">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
@@ -1387,7 +1388,7 @@
       </c>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" hidden="1">
       <c r="A36" s="3" t="s">
         <v>19</v>
       </c>
@@ -1396,7 +1397,7 @@
       </c>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" hidden="1">
       <c r="A37" s="4" t="s">
         <v>20</v>
       </c>
@@ -1405,7 +1406,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" hidden="1">
       <c r="A38" s="3" t="s">
         <v>21</v>
       </c>
@@ -1414,7 +1415,7 @@
       </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" hidden="1">
       <c r="A39" s="3" t="s">
         <v>22</v>
       </c>
@@ -1423,7 +1424,7 @@
       </c>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" hidden="1">
       <c r="A40" s="3" t="s">
         <v>23</v>
       </c>
@@ -1432,7 +1433,7 @@
       </c>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" hidden="1">
       <c r="A41" s="3" t="s">
         <v>24</v>
       </c>
@@ -1443,7 +1444,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" hidden="1">
       <c r="A42" s="3" t="s">
         <v>25</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" hidden="1">
       <c r="A43" s="3" t="s">
         <v>26</v>
       </c>
@@ -1463,7 +1464,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" hidden="1">
       <c r="A44" s="3" t="s">
         <v>27</v>
       </c>
@@ -1472,7 +1473,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" hidden="1">
       <c r="A45" s="3" t="s">
         <v>28</v>
       </c>
@@ -1481,7 +1482,7 @@
       </c>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" hidden="1">
       <c r="A46" s="3" t="s">
         <v>29</v>
       </c>
@@ -1490,7 +1491,7 @@
       </c>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" hidden="1">
       <c r="A47" s="3" t="s">
         <v>30</v>
       </c>
@@ -1499,7 +1500,7 @@
       </c>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" hidden="1">
       <c r="A48" s="3" t="s">
         <v>31</v>
       </c>
@@ -1508,7 +1509,7 @@
       </c>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" hidden="1">
       <c r="A49" s="3" t="s">
         <v>32</v>
       </c>
@@ -1517,7 +1518,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1">
+    <row r="50" spans="1:3" ht="15" hidden="1" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>33</v>
       </c>
@@ -1526,7 +1527,7 @@
       </c>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="1:3" ht="15" customHeight="1">
+    <row r="51" spans="1:3" ht="15" hidden="1" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>34</v>
       </c>
@@ -1535,7 +1536,7 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" hidden="1">
       <c r="A52" s="3" t="s">
         <v>35</v>
       </c>
@@ -1544,7 +1545,7 @@
       </c>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" hidden="1">
       <c r="A53" s="3" t="s">
         <v>36</v>
       </c>
@@ -1553,7 +1554,7 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" hidden="1">
       <c r="A54" s="3" t="s">
         <v>37</v>
       </c>
@@ -1562,7 +1563,7 @@
       </c>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" hidden="1">
       <c r="A55" s="4" t="s">
         <v>38</v>
       </c>
@@ -1571,7 +1572,7 @@
       </c>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" hidden="1">
       <c r="A56" s="4" t="s">
         <v>187</v>
       </c>
@@ -1580,7 +1581,7 @@
       </c>
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" hidden="1">
       <c r="A57" s="3" t="s">
         <v>39</v>
       </c>
@@ -1589,7 +1590,7 @@
       </c>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" hidden="1">
       <c r="A58" s="3" t="s">
         <v>40</v>
       </c>
@@ -1598,7 +1599,7 @@
       </c>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" hidden="1">
       <c r="A59" s="3" t="s">
         <v>41</v>
       </c>
@@ -1607,7 +1608,7 @@
       </c>
       <c r="C59" s="3"/>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" hidden="1">
       <c r="A60" s="3" t="s">
         <v>42</v>
       </c>
@@ -1616,7 +1617,7 @@
       </c>
       <c r="C60" s="3"/>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" hidden="1">
       <c r="A61" s="3" t="s">
         <v>43</v>
       </c>
@@ -1625,7 +1626,7 @@
       </c>
       <c r="C61" s="3"/>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" hidden="1">
       <c r="A62" s="3" t="s">
         <v>44</v>
       </c>
@@ -1634,7 +1635,7 @@
       </c>
       <c r="C62" s="3"/>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" hidden="1">
       <c r="A63" s="3" t="s">
         <v>45</v>
       </c>
@@ -1643,7 +1644,7 @@
       </c>
       <c r="C63" s="3"/>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" hidden="1">
       <c r="A64" s="3" t="s">
         <v>46</v>
       </c>
@@ -1652,7 +1653,7 @@
       </c>
       <c r="C64" s="3"/>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" hidden="1">
       <c r="A65" s="3" t="s">
         <v>47</v>
       </c>
@@ -1661,7 +1662,7 @@
       </c>
       <c r="C65" s="3"/>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" hidden="1">
       <c r="A66" s="3" t="s">
         <v>48</v>
       </c>
@@ -1670,7 +1671,7 @@
       </c>
       <c r="C66" s="3"/>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" hidden="1">
       <c r="A67" s="3" t="s">
         <v>49</v>
       </c>
@@ -1679,7 +1680,7 @@
       </c>
       <c r="C67" s="3"/>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" hidden="1">
       <c r="A68" s="3" t="s">
         <v>50</v>
       </c>
@@ -1688,7 +1689,7 @@
       </c>
       <c r="C68" s="3"/>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" hidden="1">
       <c r="A69" s="3" t="s">
         <v>51</v>
       </c>
@@ -1697,7 +1698,7 @@
       </c>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" hidden="1">
       <c r="A70" s="3" t="s">
         <v>52</v>
       </c>
@@ -1706,7 +1707,7 @@
       </c>
       <c r="C70" s="3"/>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" hidden="1">
       <c r="A71" s="3" t="s">
         <v>53</v>
       </c>
@@ -1715,7 +1716,7 @@
       </c>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" hidden="1">
       <c r="A72" s="3" t="s">
         <v>54</v>
       </c>
@@ -1724,7 +1725,7 @@
       </c>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" hidden="1">
       <c r="A73" s="3" t="s">
         <v>55</v>
       </c>
@@ -1733,7 +1734,7 @@
       </c>
       <c r="C73" s="3"/>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" hidden="1">
       <c r="A74" s="3" t="s">
         <v>56</v>
       </c>
@@ -1742,7 +1743,7 @@
       </c>
       <c r="C74" s="3"/>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" hidden="1">
       <c r="A75" s="3" t="s">
         <v>57</v>
       </c>
@@ -1751,7 +1752,7 @@
       </c>
       <c r="C75" s="3"/>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" hidden="1">
       <c r="A76" s="3" t="s">
         <v>58</v>
       </c>
@@ -1760,7 +1761,7 @@
       </c>
       <c r="C76" s="3"/>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" hidden="1">
       <c r="A77" s="3" t="s">
         <v>59</v>
       </c>
@@ -1769,7 +1770,7 @@
       </c>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" hidden="1">
       <c r="A78" s="3" t="s">
         <v>60</v>
       </c>
@@ -1778,7 +1779,7 @@
       </c>
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" hidden="1">
       <c r="A79" s="3" t="s">
         <v>61</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" hidden="1">
       <c r="A81" s="3" t="s">
         <v>63</v>
       </c>
@@ -1807,7 +1808,7 @@
       </c>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" hidden="1">
       <c r="A82" s="3" t="s">
         <v>64</v>
       </c>
@@ -1827,7 +1828,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" hidden="1">
       <c r="A84" s="3" t="s">
         <v>66</v>
       </c>
@@ -1836,7 +1837,7 @@
       </c>
       <c r="C84" s="3"/>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" hidden="1">
       <c r="A85" s="3" t="s">
         <v>67</v>
       </c>
@@ -1845,7 +1846,7 @@
       </c>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" hidden="1">
       <c r="A86" s="3" t="s">
         <v>68</v>
       </c>
@@ -1854,7 +1855,7 @@
       </c>
       <c r="C86" s="3"/>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" hidden="1">
       <c r="A87" s="3" t="s">
         <v>69</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" hidden="1">
       <c r="A89" s="3" t="s">
         <v>71</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" hidden="1">
       <c r="A91" s="3" t="s">
         <v>73</v>
       </c>
@@ -1903,7 +1904,7 @@
       </c>
       <c r="C91" s="3"/>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" hidden="1">
       <c r="A92" s="3" t="s">
         <v>74</v>
       </c>
@@ -1912,7 +1913,7 @@
       </c>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" hidden="1">
       <c r="A93" s="3" t="s">
         <v>75</v>
       </c>
@@ -1921,7 +1922,7 @@
       </c>
       <c r="C93" s="3"/>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" hidden="1">
       <c r="A94" s="4" t="s">
         <v>76</v>
       </c>
@@ -1930,7 +1931,7 @@
       </c>
       <c r="C94" s="4"/>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" hidden="1">
       <c r="A95" s="4" t="s">
         <v>157</v>
       </c>
@@ -1939,7 +1940,7 @@
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" hidden="1">
       <c r="A96" s="4" t="s">
         <v>77</v>
       </c>
@@ -1948,7 +1949,7 @@
       </c>
       <c r="C96" s="4"/>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" hidden="1">
       <c r="A97" s="3" t="s">
         <v>78</v>
       </c>
@@ -1957,7 +1958,7 @@
       </c>
       <c r="C97" s="3"/>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" hidden="1">
       <c r="A98" s="3" t="s">
         <v>79</v>
       </c>
@@ -1966,7 +1967,7 @@
       </c>
       <c r="C98" s="3"/>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" hidden="1">
       <c r="A99" s="3" t="s">
         <v>80</v>
       </c>
@@ -1975,7 +1976,7 @@
       </c>
       <c r="C99" s="3"/>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" hidden="1">
       <c r="A100" s="3" t="s">
         <v>81</v>
       </c>
@@ -1984,7 +1985,7 @@
       </c>
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" hidden="1">
       <c r="A101" s="3" t="s">
         <v>82</v>
       </c>
@@ -1993,7 +1994,7 @@
       </c>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" hidden="1">
       <c r="A102" s="3" t="s">
         <v>83</v>
       </c>
@@ -2002,7 +2003,7 @@
       </c>
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="1:3" s="7" customFormat="1">
+    <row r="103" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A103" s="3" t="s">
         <v>84</v>
       </c>
@@ -2011,7 +2012,7 @@
       </c>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="1:3" s="7" customFormat="1">
+    <row r="104" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A104" s="3" t="s">
         <v>85</v>
       </c>
@@ -2020,7 +2021,7 @@
       </c>
       <c r="C104" s="3"/>
     </row>
-    <row r="105" spans="1:3" s="7" customFormat="1">
+    <row r="105" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A105" s="4" t="s">
         <v>86</v>
       </c>
@@ -2029,7 +2030,7 @@
       </c>
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" hidden="1">
       <c r="A106" s="3" t="s">
         <v>87</v>
       </c>
@@ -2038,7 +2039,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" hidden="1">
       <c r="A107" s="3" t="s">
         <v>88</v>
       </c>
@@ -2047,7 +2048,7 @@
       </c>
       <c r="C107" s="3"/>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" hidden="1">
       <c r="A108" s="4" t="s">
         <v>89</v>
       </c>
@@ -2056,7 +2057,7 @@
       </c>
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" hidden="1">
       <c r="A109" s="3" t="s">
         <v>90</v>
       </c>
@@ -2065,7 +2066,7 @@
       </c>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" hidden="1">
       <c r="A110" s="3" t="s">
         <v>91</v>
       </c>
@@ -2074,7 +2075,7 @@
       </c>
       <c r="C110" s="3"/>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" hidden="1">
       <c r="A111" s="3" t="s">
         <v>92</v>
       </c>
@@ -2105,7 +2106,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" hidden="1">
       <c r="A114" s="3" t="s">
         <v>95</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="116" spans="1:3" s="7" customFormat="1">
+    <row r="116" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A116" s="4" t="s">
         <v>97</v>
       </c>
@@ -2134,7 +2135,7 @@
       </c>
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" hidden="1">
       <c r="A117" s="3" t="s">
         <v>98</v>
       </c>
@@ -2143,7 +2144,7 @@
       </c>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" hidden="1">
       <c r="A118" s="3" t="s">
         <v>99</v>
       </c>
@@ -2152,7 +2153,7 @@
       </c>
       <c r="C118" s="3"/>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" hidden="1">
       <c r="A119" s="3" t="s">
         <v>189</v>
       </c>
@@ -2161,7 +2162,7 @@
       </c>
       <c r="C119" s="3"/>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" hidden="1">
       <c r="A120" s="3" t="s">
         <v>100</v>
       </c>
@@ -2170,7 +2171,7 @@
       </c>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" hidden="1">
       <c r="A121" s="3" t="s">
         <v>101</v>
       </c>
@@ -2179,7 +2180,7 @@
       </c>
       <c r="C121" s="3"/>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" hidden="1">
       <c r="A122" s="3" t="s">
         <v>102</v>
       </c>
@@ -2188,7 +2189,7 @@
       </c>
       <c r="C122" s="3"/>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" hidden="1">
       <c r="A123" s="3" t="s">
         <v>103</v>
       </c>
@@ -2197,7 +2198,7 @@
       </c>
       <c r="C123" s="3"/>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" hidden="1">
       <c r="A124" s="3" t="s">
         <v>104</v>
       </c>
@@ -2206,7 +2207,7 @@
       </c>
       <c r="C124" s="3"/>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" hidden="1">
       <c r="A125" s="3" t="s">
         <v>105</v>
       </c>
@@ -2215,7 +2216,7 @@
       </c>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" hidden="1">
       <c r="A126" s="3" t="s">
         <v>106</v>
       </c>
@@ -2224,7 +2225,7 @@
       </c>
       <c r="C126" s="3"/>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" hidden="1">
       <c r="A127" s="3" t="s">
         <v>107</v>
       </c>
@@ -2233,7 +2234,7 @@
       </c>
       <c r="C127" s="3"/>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" hidden="1">
       <c r="A128" s="3" t="s">
         <v>108</v>
       </c>
@@ -2242,7 +2243,7 @@
       </c>
       <c r="C128" s="3"/>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" hidden="1">
       <c r="A129" s="3" t="s">
         <v>109</v>
       </c>
@@ -2251,7 +2252,7 @@
       </c>
       <c r="C129" s="3"/>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" hidden="1">
       <c r="A130" s="3" t="s">
         <v>110</v>
       </c>
@@ -2260,7 +2261,7 @@
       </c>
       <c r="C130" s="3"/>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" hidden="1">
       <c r="A131" s="3" t="s">
         <v>111</v>
       </c>
@@ -2291,7 +2292,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" hidden="1">
       <c r="A134" s="3" t="s">
         <v>114</v>
       </c>
@@ -2300,7 +2301,7 @@
       </c>
       <c r="C134" s="3"/>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" hidden="1">
       <c r="A135" s="3" t="s">
         <v>115</v>
       </c>
@@ -2322,7 +2323,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" hidden="1">
       <c r="A137" s="3" t="s">
         <v>117</v>
       </c>
@@ -2333,7 +2334,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" hidden="1">
       <c r="A138" s="3" t="s">
         <v>118</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" hidden="1">
       <c r="A139" s="3" t="s">
         <v>119</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" hidden="1">
       <c r="A140" s="3" t="s">
         <v>120</v>
       </c>
@@ -2366,7 +2367,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" hidden="1">
       <c r="A141" s="3" t="s">
         <v>121</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" hidden="1">
       <c r="A142" s="3" t="s">
         <v>122</v>
       </c>
@@ -2388,7 +2389,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" hidden="1">
       <c r="A143" s="4" t="s">
         <v>123</v>
       </c>
@@ -2399,7 +2400,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" hidden="1">
       <c r="A144" s="4" t="s">
         <v>124</v>
       </c>
@@ -2410,7 +2411,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" hidden="1">
       <c r="A145" s="4" t="s">
         <v>125</v>
       </c>
@@ -2421,7 +2422,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" hidden="1">
       <c r="A146" s="4" t="s">
         <v>126</v>
       </c>
@@ -2432,7 +2433,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" hidden="1">
       <c r="A147" s="3" t="s">
         <v>127</v>
       </c>
@@ -2443,7 +2444,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="148" spans="1:3" s="7" customFormat="1">
+    <row r="148" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A148" s="3" t="s">
         <v>128</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="149" spans="1:3" s="7" customFormat="1">
+    <row r="149" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A149" s="3" t="s">
         <v>129</v>
       </c>
@@ -2465,7 +2466,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="150" spans="1:3" s="7" customFormat="1">
+    <row r="150" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A150" s="3" t="s">
         <v>130</v>
       </c>
@@ -2476,7 +2477,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="151" spans="1:3" s="7" customFormat="1">
+    <row r="151" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A151" s="3" t="s">
         <v>131</v>
       </c>
@@ -2487,7 +2488,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" hidden="1">
       <c r="A152" s="4" t="s">
         <v>132</v>
       </c>
@@ -2498,7 +2499,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" hidden="1">
       <c r="A153" s="3" t="s">
         <v>133</v>
       </c>
@@ -2509,7 +2510,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" hidden="1">
       <c r="A154" s="3" t="s">
         <v>134</v>
       </c>
@@ -2520,7 +2521,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" hidden="1">
       <c r="A155" s="3" t="s">
         <v>135</v>
       </c>
@@ -2531,7 +2532,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" hidden="1">
       <c r="A156" s="3" t="s">
         <v>136</v>
       </c>
@@ -2542,7 +2543,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" hidden="1">
       <c r="A157" s="4" t="s">
         <v>137</v>
       </c>
@@ -2553,7 +2554,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" hidden="1">
       <c r="A158" s="3" t="s">
         <v>138</v>
       </c>
@@ -2564,7 +2565,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="159" spans="1:3" s="7" customFormat="1">
+    <row r="159" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A159" s="3" t="s">
         <v>139</v>
       </c>
@@ -2575,7 +2576,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="160" spans="1:3" s="7" customFormat="1">
+    <row r="160" spans="1:3" s="7" customFormat="1" hidden="1">
       <c r="A160" s="3" t="s">
         <v>140</v>
       </c>
@@ -2586,7 +2587,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" hidden="1">
       <c r="A161" s="4" t="s">
         <v>141</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" hidden="1">
       <c r="A162" s="3" t="s">
         <v>142</v>
       </c>
@@ -2608,7 +2609,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" hidden="1">
       <c r="A163" s="4" t="s">
         <v>143</v>
       </c>
@@ -2619,7 +2620,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" hidden="1">
       <c r="A164" s="3" t="s">
         <v>144</v>
       </c>
@@ -2630,7 +2631,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" hidden="1">
       <c r="A165" s="4" t="s">
         <v>145</v>
       </c>
@@ -2641,7 +2642,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" hidden="1">
       <c r="A166" s="3" t="s">
         <v>146</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" hidden="1">
       <c r="A167" s="4" t="s">
         <v>147</v>
       </c>
@@ -2663,7 +2664,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" hidden="1">
       <c r="A168" s="3" t="s">
         <v>148</v>
       </c>
@@ -2674,7 +2675,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" hidden="1">
       <c r="A169" s="3" t="s">
         <v>149</v>
       </c>
@@ -2685,7 +2686,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" hidden="1">
       <c r="A170" s="3" t="s">
         <v>150</v>
       </c>
@@ -2696,7 +2697,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" hidden="1">
       <c r="A171" s="3" t="s">
         <v>151</v>
       </c>
@@ -2707,7 +2708,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" hidden="1">
       <c r="A172" s="3" t="s">
         <v>152</v>
       </c>
@@ -2718,7 +2719,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" hidden="1">
       <c r="A173" s="3" t="s">
         <v>153</v>
       </c>
@@ -2729,7 +2730,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" hidden="1">
       <c r="A174" s="4" t="s">
         <v>190</v>
       </c>
@@ -2740,7 +2741,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" hidden="1">
       <c r="A175" s="3" t="s">
         <v>154</v>
       </c>
@@ -2751,7 +2752,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" hidden="1">
       <c r="A176" s="3" t="s">
         <v>155</v>
       </c>
@@ -2762,7 +2763,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" hidden="1">
       <c r="A177" s="4" t="s">
         <v>156</v>
       </c>
@@ -4924,7 +4925,13 @@
       <c r="C607"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C177" xr:uid="{F0F1E9AA-42FA-48CE-9C0D-6753CE8DE448}"/>
+  <autoFilter ref="A1:C177" xr:uid="{F0F1E9AA-42FA-48CE-9C0D-6753CE8DE448}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="stage_1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C1048576" xr:uid="{282CD8DC-1CD6-4FEE-88BD-6500CF45AFA3}">
       <formula1>"#na, stage_1, stage_2, stage_3, stage_4, stage_5, stage_6, stage_7, stage_8, stage_9, stage_10, stage_11, stage_12, stage_13"</formula1>

</xml_diff>